<commit_message>
add boms add swd adapter
</commit_message>
<xml_diff>
--- a/HW/Project Outputs for btalti/btalti.xlsx
+++ b/HW/Project Outputs for btalti/btalti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\bt_alti\HW\Project Outputs for btalti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AB7B1E1-0F96-432B-BA1F-C374CACD5F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E96B22CA-795D-4FC8-8877-5056425AD8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12645" xr2:uid="{31A728EF-7856-440D-840F-5E4E2C8FA37D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1CB65EFF-2EDA-473C-92D1-B2A77A9DD3CF}"/>
   </bookViews>
   <sheets>
     <sheet name="btalti" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="222">
   <si>
     <t>Comment</t>
   </si>
@@ -59,18 +59,15 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Fabricant</t>
+  </si>
+  <si>
+    <t>Référence</t>
+  </si>
+  <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Fabriquant</t>
-  </si>
-  <si>
-    <t>Fabricant</t>
-  </si>
-  <si>
-    <t>Référence</t>
-  </si>
-  <si>
     <t>2450AT42E0100</t>
   </si>
   <si>
@@ -80,12 +77,12 @@
     <t>A1</t>
   </si>
   <si>
+    <t>PulseLarsen Antennas</t>
+  </si>
+  <si>
     <t>50_OHMS</t>
   </si>
   <si>
-    <t>PulseLarsen Antennas</t>
-  </si>
-  <si>
     <t>EC382704P-T</t>
   </si>
   <si>
@@ -122,87 +119,87 @@
     <t>Omron</t>
   </si>
   <si>
+    <t>1uF (0402) AEC-Q200</t>
+  </si>
+  <si>
+    <t>X7S 10% 0402 10V AEC-Q200</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GCM155C71A105KE38D</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>100nF (0402) AEC-Q200</t>
+  </si>
+  <si>
+    <t>X7R 0402 10% 50V AEC-Q200</t>
+  </si>
+  <si>
+    <t>C9, C11, C13, C15, C16, C19, C21, C22, C35, C36</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>GCM155R71H104KE02J</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>4.7uF (0402) AEC-Q200</t>
+  </si>
+  <si>
+    <t>X7T 0402 10% 6.3V AEC-Q200</t>
+  </si>
+  <si>
+    <t>C10, C17, C18, C42</t>
+  </si>
+  <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
+    <t>KAM05CT70J475KH</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
     <t>1uF (0402)</t>
   </si>
   <si>
     <t>X7S 10% 0402 16V</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C12, C29, C30, C31, C32, C33, C34</t>
-  </si>
-  <si>
-    <t>C0402</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>MURATA</t>
+    <t>C12, C29, C30, C31, C32, C33, C34</t>
   </si>
   <si>
     <t>GRM155C71C105KE11D</t>
   </si>
   <si>
-    <t>100nF (0402)</t>
-  </si>
-  <si>
-    <t>X7R 0402 20% 50V</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>C1005X7R1H104M050BB</t>
-  </si>
-  <si>
-    <t>4.7uF (0402) AEC-Q200</t>
-  </si>
-  <si>
-    <t>X7T 0402 20% 6.3V AEC-Q200, X7T 0402 10% 6.3V AEC-Q200</t>
-  </si>
-  <si>
-    <t>C10, C17, C18, C42</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>Murata, KYOCERA AVX</t>
-  </si>
-  <si>
-    <t>GRT155D70J475ME13J, KAM05CT70J475KH</t>
-  </si>
-  <si>
-    <t>100nF (0402) AEC-Q200</t>
-  </si>
-  <si>
-    <t>X7R 0402 10% 50V AEC-Q200</t>
-  </si>
-  <si>
-    <t>C11, C13, C15, C16, C19, C21, C22, C35, C36</t>
-  </si>
-  <si>
-    <t>GCM155R71H104KE02J</t>
-  </si>
-  <si>
     <t>10nF (0402) AEC-Q200</t>
   </si>
   <si>
     <t>C14</t>
   </si>
   <si>
+    <t>GRT155R71H103KE01D</t>
+  </si>
+  <si>
     <t>10nF</t>
   </si>
   <si>
-    <t>GRT155R71H103KE01D</t>
-  </si>
-  <si>
     <t>100pF (0402) AEC-Q200</t>
   </si>
   <si>
@@ -212,12 +209,12 @@
     <t>C20</t>
   </si>
   <si>
+    <t>GCM1555C1H101JA16D</t>
+  </si>
+  <si>
     <t>100pF</t>
   </si>
   <si>
-    <t>GCM1555C1H101JA16D</t>
-  </si>
-  <si>
     <t>NM (0402)</t>
   </si>
   <si>
@@ -227,7 +224,7 @@
     <t>C0402 (NM)</t>
   </si>
   <si>
-    <t>20nF, NM</t>
+    <t>NM</t>
   </si>
   <si>
     <t>5.1pF (0402) AEC-Q200</t>
@@ -236,12 +233,12 @@
     <t>C27, C28</t>
   </si>
   <si>
+    <t>GCM1555C1H5R1CA16D</t>
+  </si>
+  <si>
     <t>5.1pF</t>
   </si>
   <si>
-    <t>GCM1555C1H5R1CA16D</t>
-  </si>
-  <si>
     <t>1uF (0402) AEC-Q200 HT</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
   </si>
   <si>
     <t>C37, C38, C39, C40, C41, C43, C44, C45, C46</t>
-  </si>
-  <si>
-    <t>Murata</t>
   </si>
   <si>
     <t>GRT155C81E105KE13D</t>
@@ -319,13 +313,13 @@
     <t>SOD-882 (0402)</t>
   </si>
   <si>
+    <t>NEXPERIA</t>
+  </si>
+  <si>
+    <t>PMEG4002EL,315</t>
+  </si>
+  <si>
     <t>Schottky</t>
-  </si>
-  <si>
-    <t>NEXPERIA</t>
-  </si>
-  <si>
-    <t>PMEG4002EL,315</t>
   </si>
   <si>
     <t>MLPF-WB55-01E3</t>
@@ -452,15 +446,15 @@
     <t>2.5x2 (2512)</t>
   </si>
   <si>
+    <t>WURTH ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>74404024100</t>
+  </si>
+  <si>
     <t>10uH</t>
   </si>
   <si>
-    <t>WURTH ELEKTRONIK</t>
-  </si>
-  <si>
-    <t>74404024100</t>
-  </si>
-  <si>
     <t>4.7uH (0603)</t>
   </si>
   <si>
@@ -473,24 +467,21 @@
     <t>S0603</t>
   </si>
   <si>
+    <t>COILCRAFT</t>
+  </si>
+  <si>
+    <t>PFL1609-472MEU</t>
+  </si>
+  <si>
     <t>4.7uH</t>
   </si>
   <si>
-    <t>COILCRAFT</t>
-  </si>
-  <si>
-    <t>PFL1609-472MEU</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
     <t>S0402 (NM)</t>
   </si>
   <si>
-    <t>NM</t>
-  </si>
-  <si>
     <t>ECS-320-8-47Q-CES-TR</t>
   </si>
   <si>
@@ -503,15 +494,15 @@
     <t>2.0x1.6 - ECS-320-8-47Q</t>
   </si>
   <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>ECS-320-10-37Q-ES-TR</t>
+  </si>
+  <si>
     <t>32MHz</t>
   </si>
   <si>
-    <t>ECS Inc.</t>
-  </si>
-  <si>
-    <t>ECS-320-10-37Q-ES-TR</t>
-  </si>
-  <si>
     <t>ECS-.327-12.5-34QCS-TR</t>
   </si>
   <si>
@@ -524,12 +515,12 @@
     <t>3.2x1.5</t>
   </si>
   <si>
+    <t>ECS</t>
+  </si>
+  <si>
     <t>32.768k</t>
   </si>
   <si>
-    <t>ECS</t>
-  </si>
-  <si>
     <t>1k (0402)</t>
   </si>
   <si>
@@ -542,51 +533,51 @@
     <t>R0402</t>
   </si>
   <si>
+    <t>MULTICOMP</t>
+  </si>
+  <si>
+    <t>MCWR04X1001FTL</t>
+  </si>
+  <si>
     <t>1k</t>
   </si>
   <si>
-    <t>MULTICOMP</t>
-  </si>
-  <si>
-    <t>MCWR04X1001FTL</t>
-  </si>
-  <si>
     <t>10k (0402)</t>
   </si>
   <si>
     <t>R2, R7, R17, R19, R20, R21</t>
   </si>
   <si>
+    <t>MCWR04X1002FTL</t>
+  </si>
+  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>MCWR04X1002FTL</t>
-  </si>
-  <si>
     <t>1M (0402)</t>
   </si>
   <si>
     <t>R3, R10</t>
   </si>
   <si>
+    <t>MCWR04X1004FTL</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
-    <t>MCWR04X1004FTL</t>
-  </si>
-  <si>
     <t>47k (0402)</t>
   </si>
   <si>
     <t>R4</t>
   </si>
   <si>
+    <t>MCWR04X4702FTL</t>
+  </si>
+  <si>
     <t>47k</t>
   </si>
   <si>
-    <t>MCWR04X4702FTL</t>
-  </si>
-  <si>
     <t>5k1 (0402) AEC-Q200</t>
   </si>
   <si>
@@ -596,15 +587,15 @@
     <t>R8, R9</t>
   </si>
   <si>
+    <t>PANASONIC</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF5101X</t>
+  </si>
+  <si>
     <t>5k1</t>
   </si>
   <si>
-    <t>PANASONIC</t>
-  </si>
-  <si>
-    <t>ERJ-2RKF5101X</t>
-  </si>
-  <si>
     <t>100k (0402)</t>
   </si>
   <si>
@@ -614,12 +605,12 @@
     <t>R11, R12</t>
   </si>
   <si>
+    <t>MCWR04X1003FTL</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
-    <t>MCWR04X1003FTL</t>
-  </si>
-  <si>
     <t>R13, R18</t>
   </si>
   <si>
@@ -644,12 +635,12 @@
     <t>R22</t>
   </si>
   <si>
+    <t>ERJ-U020R00X</t>
+  </si>
+  <si>
     <t>0R</t>
   </si>
   <si>
-    <t>ERJ-U020R00X</t>
-  </si>
-  <si>
     <t>2R2 (0402)</t>
   </si>
   <si>
@@ -659,15 +650,15 @@
     <t>R23</t>
   </si>
   <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>AC0402FR-072R2L</t>
+  </si>
+  <si>
     <t>2R2</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
-    <t>AC0402FR-072R2L</t>
-  </si>
-  <si>
     <t>Ferrite (0402) 1k AEC-Q200</t>
   </si>
   <si>
@@ -680,10 +671,13 @@
     <t>0402 (FERRITE)</t>
   </si>
   <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MMZ1005Y102CTD25</t>
+  </si>
+  <si>
     <t>Ferrite</t>
-  </si>
-  <si>
-    <t>MMZ1005Y102CTD25</t>
   </si>
   <si>
     <t>BS170F</t>
@@ -1112,18 +1106,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25251CB8-9C4C-497A-B91C-02EF051E8F11}">
-  <dimension ref="A1:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD96B63-6C0F-41B9-B5D7-8E09AFB47FA6}">
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
-    <col min="7" max="10" width="16.7109375" customWidth="1"/>
+    <col min="7" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1151,1304 +1145,1257 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1">
-        <v>15</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1">
         <v>5</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="I14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F18" s="1">
         <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="I21" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H23" s="1"/>
       <c r="I23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="I24" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="I25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="I26" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="H27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="H32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F33" s="1">
         <v>3</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F34" s="1">
         <v>6</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F35" s="1">
         <v>2</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J35" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F37" s="1">
         <v>2</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F38" s="1">
         <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F39" s="1">
         <v>2</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>148</v>
-      </c>
+      <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F40" s="1">
-        <v>1</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="E43" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F44" s="1">
         <v>2</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H44" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="I44" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="H45" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="J45" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>